<commit_message>
added mycol lectures 5,6
</commit_message>
<xml_diff>
--- a/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
+++ b/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Faculty mentor</t>
   </si>
@@ -37,6 +37,18 @@
     <t xml:space="preserve">Rating</t>
   </si>
   <si>
+    <t xml:space="preserve">Fall 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Britt Wyatt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Britt.Wyatt@uvu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1q7T838XMKfFK47juhkcxBeVi-VsfZCxK/view?usp=sharing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lauren Brooks </t>
   </si>
   <si>
@@ -76,7 +88,7 @@
     <t xml:space="preserve">gazdikmi@uvu.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">https://bit.ly/2Ktvhdm</t>
+    <t xml:space="preserve">https://youtu.be/_hHyhnSjnCI</t>
   </si>
   <si>
     <t xml:space="preserve">Olga Kopp </t>
@@ -115,7 +127,7 @@
     <t xml:space="preserve">gzahn@uvu.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">https://bit.ly/2ZRIcuR</t>
+    <t xml:space="preserve">https://youtu.be/bV967wX54Mk</t>
   </si>
   <si>
     <t xml:space="preserve">Alma Laney</t>
@@ -134,14 +146,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,17 +177,28 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -234,6 +259,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,14 +272,34 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,198 +320,229 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.53061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="2" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="H2" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="H7" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="H9" s="10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="30.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+      <c r="E12" s="6"/>
+      <c r="H12" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="30.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="https://bit.ly/2Tn9rea"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://bit.ly/2H3iCf0"/>
-    <hyperlink ref="D5" r:id="rId3" display="https://bit.ly/2MTERHX"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://bit.ly/2Ktvhdm"/>
-    <hyperlink ref="D7" r:id="rId5" display="https://bit.ly/2YZ7J42"/>
-    <hyperlink ref="D8" r:id="rId6" display="https://bit.ly/2KDTzjG"/>
-    <hyperlink ref="D11" r:id="rId7" display="https://bit.ly/2ZRIcuR"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://drive.google.com/file/d/1q7T838XMKfFK47juhkcxBeVi-VsfZCxK/view?usp=sharing"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://bit.ly/2Tn9rea"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://bit.ly/2H3iCf0"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://bit.ly/2MTERHX"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://youtu.be/_hHyhnSjnCI"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://bit.ly/2YZ7J42"/>
+    <hyperlink ref="D9" r:id="rId7" display="https://bit.ly/2KDTzjG"/>
+    <hyperlink ref="D12" r:id="rId8" display="https://youtu.be/bV967wX54Mk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
faculty mentor list update
</commit_message>
<xml_diff>
--- a/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
+++ b/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Faculty mentor</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Rating</t>
   </si>
   <si>
-    <t xml:space="preserve">Fall 2020</t>
+    <t xml:space="preserve">1=First choice</t>
   </si>
   <si>
     <t xml:space="preserve">Britt Wyatt</t>
@@ -76,22 +76,13 @@
     <t xml:space="preserve">https://youtu.be/TsbR8sEKxlc</t>
   </si>
   <si>
-    <t xml:space="preserve">Paul Dunn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul.Dunn@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://bit.ly/2Tn9rea</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eric Domyan </t>
   </si>
   <si>
     <t xml:space="preserve">Eric.Domyan@uvu.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">https://bit.ly/2H3iCf0</t>
+    <t xml:space="preserve">https://youtu.be/mVu7Hr2MwWo</t>
   </si>
   <si>
     <t xml:space="preserve">Heath Ogden </t>
@@ -112,24 +103,6 @@
     <t xml:space="preserve">https://youtu.be/_hHyhnSjnCI</t>
   </si>
   <si>
-    <t xml:space="preserve">Olga Kopp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOPPOL@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://bit.ly/2YZ7J42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erin Riggs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">erin.riggs@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://bit.ly/2KDTzjG</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sebastien Tauzin </t>
   </si>
   <si>
@@ -145,6 +118,18 @@
     <t xml:space="preserve">Danielle.Taylor@uvu.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">https://youtu.be/qqC5Be2AjUk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin Taylor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin.Taylor@uvu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/qgyWO9_ryK0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Geoffrey Zahn</t>
   </si>
   <si>
@@ -152,18 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/bV967wX54Mk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alma Laney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALaney@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kristin DeNesnera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kdenesnera@uvu.edu</t>
   </si>
 </sst>
 </file>
@@ -174,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,13 +178,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -285,7 +251,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,7 +279,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,10 +300,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,9 +311,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="65.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
   </cols>
@@ -368,9 +335,10 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -384,10 +352,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="H2" s="10" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -401,9 +366,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="H3" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -417,9 +380,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="H4" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -433,9 +394,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="H5" s="10" t="b">
-        <v>1</v>
-      </c>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -449,6 +408,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="6"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -462,6 +422,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="6"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
@@ -475,10 +436,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="H8" s="10" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
@@ -492,10 +450,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="H9" s="10" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
@@ -509,6 +464,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="6"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
@@ -522,12 +478,9 @@
         <v>35</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="H11" s="10" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
@@ -539,59 +492,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="H12" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="H14" s="10" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="27.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="30.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="6"/>
+      <c r="H12" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -599,14 +500,13 @@
     <hyperlink ref="D3" r:id="rId2" display="https://youtu.be/dIf4OAH8OAg"/>
     <hyperlink ref="D4" r:id="rId3" display="https://youtu.be/HzzFVlR_YJc"/>
     <hyperlink ref="D5" r:id="rId4" display="https://youtu.be/TsbR8sEKxlc"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://bit.ly/2Tn9rea"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://bit.ly/2H3iCf0"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://youtu.be/UF3YN6AlC9A"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://youtu.be/_hHyhnSjnCI"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://bit.ly/2YZ7J42"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://bit.ly/2KDTzjG"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://youtu.be/g76wkaXugd8"/>
-    <hyperlink ref="D14" r:id="rId12" display="https://youtu.be/bV967wX54Mk"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://youtu.be/mVu7Hr2MwWo"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://youtu.be/UF3YN6AlC9A"/>
+    <hyperlink ref="D8" r:id="rId7" display="https://youtu.be/_hHyhnSjnCI"/>
+    <hyperlink ref="D9" r:id="rId8" display="https://youtu.be/g76wkaXugd8"/>
+    <hyperlink ref="D10" r:id="rId9" display="https://youtu.be/qqC5Be2AjUk"/>
+    <hyperlink ref="D11" r:id="rId10" display="https://youtu.be/qgyWO9_ryK0"/>
+    <hyperlink ref="D12" r:id="rId11" display="https://youtu.be/bV967wX54Mk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add faculty mentor info for SSTEM
</commit_message>
<xml_diff>
--- a/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
+++ b/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">Faculty mentor</t>
   </si>
@@ -31,12 +31,15 @@
     <t xml:space="preserve">Research Area</t>
   </si>
   <si>
+    <t xml:space="preserve">Intro Video / Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Rating</t>
-  </si>
-  <si>
     <t xml:space="preserve">1=First choice</t>
   </si>
   <si>
@@ -58,24 +61,6 @@
     <t xml:space="preserve">https://youtu.be/dIf4OAH8OAg</t>
   </si>
   <si>
-    <t xml:space="preserve">Ashley Egan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aegan@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://youtu.be/HzzFVlR_YJc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lauren Brooks </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lauren.Brooks@uvu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://youtu.be/TsbR8sEKxlc</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eric Domyan </t>
   </si>
   <si>
@@ -121,6 +106,9 @@
     <t xml:space="preserve">https://youtu.be/qqC5Be2AjUk</t>
   </si>
   <si>
+    <t xml:space="preserve">often requires weekends and evenings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Devin Taylor</t>
   </si>
   <si>
@@ -137,6 +125,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/bV967wX54Mk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carl Hjelmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cehjelmen@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cehjelmen.github.io/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jess Cusick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JCusick@uvu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.jessicacusick.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Dunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul.Dunn@uvu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVU Directory Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alma Laney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALaney@uvu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://almalaney.wixsite.com/aglaney</t>
   </si>
 </sst>
 </file>
@@ -147,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -179,6 +203,13 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -234,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,6 +312,18 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -300,10 +343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,10 +356,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="65.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -335,178 +379,211 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="H2" s="10"/>
+      <c r="F2" s="7"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
+      <c r="F3" s="7"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="H4" s="10"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0"/>
+        <v>17</v>
+      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="H5" s="10"/>
+      <c r="F5" s="6"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="H6" s="10"/>
+      <c r="F6" s="6"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="H7" s="10"/>
+      <c r="F7" s="6"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="H8" s="10"/>
+      <c r="F8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F9" s="6"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="11" t="s">
+      <c r="F10" s="0"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="D11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="11" t="s">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="H12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://drive.google.com/file/d/1q7T838XMKfFK47juhkcxBeVi-VsfZCxK/view?usp=sharing"/>
     <hyperlink ref="D3" r:id="rId2" display="https://youtu.be/dIf4OAH8OAg"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://youtu.be/HzzFVlR_YJc"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://youtu.be/TsbR8sEKxlc"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://youtu.be/mVu7Hr2MwWo"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://youtu.be/UF3YN6AlC9A"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://youtu.be/_hHyhnSjnCI"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://youtu.be/g76wkaXugd8"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://youtu.be/qqC5Be2AjUk"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://youtu.be/qgyWO9_ryK0"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://youtu.be/bV967wX54Mk"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://youtu.be/mVu7Hr2MwWo"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://youtu.be/UF3YN6AlC9A"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://youtu.be/_hHyhnSjnCI"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://youtu.be/g76wkaXugd8"/>
+    <hyperlink ref="D8" r:id="rId7" display="https://youtu.be/qqC5Be2AjUk"/>
+    <hyperlink ref="D9" r:id="rId8" display="https://youtu.be/qgyWO9_ryK0"/>
+    <hyperlink ref="D10" r:id="rId9" display="https://youtu.be/bV967wX54Mk"/>
+    <hyperlink ref="D11" r:id="rId10" display="https://cehjelmen.github.io/"/>
+    <hyperlink ref="D12" r:id="rId11" display="https://www.jessicacusick.com/"/>
+    <hyperlink ref="D13" r:id="rId12" display="UVU Directory Page"/>
+    <hyperlink ref="D14" r:id="rId13" display="https://almalaney.wixsite.com/aglaney"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update video links for mentor intros
</commit_message>
<xml_diff>
--- a/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
+++ b/SSTEM/media/Research_Mentor_Ranking_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">Faculty mentor</t>
   </si>
@@ -34,15 +34,13 @@
     <t xml:space="preserve">Intro Video / Info</t>
   </si>
   <si>
-    <t xml:space="preserve">Rating</t>
+    <t xml:space="preserve">Rating
+1 = first choice</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">1=First choice</t>
-  </si>
-  <si>
     <t xml:space="preserve">Britt Wyatt</t>
   </si>
   <si>
@@ -142,7 +140,8 @@
     <t xml:space="preserve">JCusick@uvu.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.jessicacusick.com/</t>
+    <t xml:space="preserve">https://www.jessicacusick.com/
+https://drive.google.com/file/d/1Y3h5iC8Yp2x9rgiLD5bPKDzFl_sMs-25/view?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Paul Dunn</t>
@@ -202,7 +201,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="8"/>
+      <sz val="9"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -282,6 +281,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,56 +317,52 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="65.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="74.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.93"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -376,198 +375,206 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" s="10" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" s="10" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" s="9" customFormat="true" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12" t="s">
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="32.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="0"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -581,9 +588,8 @@
     <hyperlink ref="D9" r:id="rId8" display="https://youtu.be/qgyWO9_ryK0"/>
     <hyperlink ref="D10" r:id="rId9" display="https://youtu.be/bV967wX54Mk"/>
     <hyperlink ref="D11" r:id="rId10" display="https://cehjelmen.github.io/"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://www.jessicacusick.com/"/>
-    <hyperlink ref="D13" r:id="rId12" display="UVU Directory Page"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://almalaney.wixsite.com/aglaney"/>
+    <hyperlink ref="D13" r:id="rId11" display="UVU Directory Page"/>
+    <hyperlink ref="D14" r:id="rId12" display="https://almalaney.wixsite.com/aglaney"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>